<commit_message>
Simulation results are now summarized by a structure that is independent of the rest of the project (so they can be snapshotted later)
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{436A1BB7-9AAC-4945-9ABA-E2FB07F59370}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BABE5E-7C7E-4E69-9B0D-F9A118510F03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5310" yWindow="1815" windowWidth="16905" windowHeight="8280" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
@@ -31,6 +31,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>LNP</t>
+  </si>
+  <si>
+    <t>ALP</t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t>ONP</t>
+  </si>
+  <si>
+    <t>NXT</t>
+  </si>
+  <si>
+    <t>UAP</t>
+  </si>
+  <si>
+    <t>OTH</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,69 +408,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>45.1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>34.1</v>
-      </c>
-      <c r="C1" s="2">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E1" s="2" t="e">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F1" s="2" t="e">
+      <c r="F2" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G1" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="I1">
-        <f>SUMIF(A1:G1,"&gt;0")</f>
-        <v>100.10000000000001</v>
+      <c r="G2" s="2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <f>SUMIF(A2:G2,"&gt;0")</f>
+        <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>A1*100/$I$1</f>
-        <v>45.054945054945051</v>
-      </c>
-      <c r="B3" s="1">
-        <f t="shared" ref="B3:G3" si="0">B1*100/$I$1</f>
-        <v>34.065934065934066</v>
-      </c>
-      <c r="C3" s="1">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A2*100/$I$2</f>
+        <v>40.217391304347828</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:G4" si="0">B2*100/$I$2</f>
+        <v>38.043478260869563</v>
+      </c>
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>10.989010989010987</v>
-      </c>
-      <c r="D3" s="1">
+        <v>10.869565217391305</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>4.395604395604396</v>
-      </c>
-      <c r="E3" s="1" t="e">
+        <v>3.2608695652173911</v>
+      </c>
+      <c r="E4" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F3" s="1" t="e">
+      <c r="F4" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>5.4945054945054936</v>
+        <v>7.6086956521739131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Essential and ResolvePM
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BABE5E-7C7E-4E69-9B0D-F9A118510F03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B705BC-EF6F-463B-8095-DCF0544ED8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="1815" windowWidth="16905" windowHeight="8280" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="6225" yWindow="9705" windowWidth="17700" windowHeight="11820" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>LNP</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +441,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2">
         <v>35</v>
@@ -450,50 +450,70 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2" s="2" t="e">
-        <v>#N/A</v>
+      <c r="F2" s="2">
+        <v>1</v>
       </c>
       <c r="G2" s="2">
         <v>7</v>
       </c>
       <c r="I2">
         <f>SUMIF(A2:G2,"&gt;0")</f>
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$I$2</f>
-        <v>40.217391304347828</v>
+        <v>38.297872340425535</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:G4" si="0">B2*100/$I$2</f>
-        <v>38.043478260869563</v>
+        <v>37.234042553191486</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>10.869565217391305</v>
+        <v>10.638297872340425</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>3.2608695652173911</v>
+        <v>5.3191489361702127</v>
       </c>
       <c r="E4" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4" s="1" t="e">
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>7.6086956521739131</v>
+        <v>7.4468085106382977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f>SUM(A9:B9)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script for sending uploads fully functional
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B705BC-EF6F-463B-8095-DCF0544ED8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE2127F-1F53-4BEA-82FA-8463550DC952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="9705" windowWidth="17700" windowHeight="11820" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="24240" yWindow="4245" windowWidth="18795" windowHeight="16710" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>LNP</t>
   </si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>OTH</t>
+  </si>
+  <si>
+    <t>copy^</t>
   </si>
 </sst>
 </file>
@@ -408,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,6 +520,26 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f>A9*100/D8</f>
+        <v>51.612903225806448</v>
+      </c>
+      <c r="B10" s="2">
+        <f>B9*100/D8</f>
+        <v>48.387096774193552</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Morgan + Essential polls.
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git repositories\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE2127F-1F53-4BEA-82FA-8463550DC952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699DD9C9-8400-4FEA-A69F-46420C323137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="4245" windowWidth="18795" windowHeight="16710" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="16230" yWindow="4260" windowWidth="19905" windowHeight="11160" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -415,7 +414,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,47 +444,47 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2">
         <v>35</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="e">
         <v>#N/A</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <f>SUMIF(A2:G2,"&gt;0")</f>
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$I$2</f>
-        <v>38.297872340425535</v>
+        <v>39.784946236559136</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:G4" si="0">B2*100/$I$2</f>
-        <v>37.234042553191486</v>
+        <v>37.634408602150536</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>10.638297872340425</v>
+        <v>9.67741935483871</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>5.3191489361702127</v>
+        <v>3.225806451612903</v>
       </c>
       <c r="E4" s="1" t="e">
         <f t="shared" si="0"/>
@@ -493,11 +492,11 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1.0638297872340425</v>
+        <v>4.301075268817204</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>7.4468085106382977</v>
+        <v>5.376344086021505</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -509,25 +508,25 @@
       </c>
       <c r="D8">
         <f>SUM(A9:B9)</f>
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>44</v>
+      </c>
+      <c r="B9">
         <v>48</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>A9*100/D8</f>
-        <v>51.612903225806448</v>
+        <v>47.826086956521742</v>
       </c>
       <c r="B10" s="2">
         <f>B9*100/D8</f>
-        <v>48.387096774193552</v>
+        <v>52.173913043478258</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ind preferencing sheet with SA results
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git repositories\Polling Analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699DD9C9-8400-4FEA-A69F-46420C323137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDE46B8-4F53-4C14-9726-3DFAF2DE2194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16230" yWindow="4260" windowWidth="19905" windowHeight="11160" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="18600" yWindow="5880" windowWidth="19800" windowHeight="14055" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>LNP</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>copy^</t>
+  </si>
+  <si>
+    <t>DEM</t>
   </si>
 </sst>
 </file>
@@ -411,15 +414,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -439,52 +445,58 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="e">
         <v>#N/A</v>
       </c>
       <c r="F2" s="2">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <f>SUMIF(A2:G2,"&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2" s="2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <f>SUMIF(A2:H2,"&gt;0")</f>
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A2*100/$I$2</f>
-        <v>39.784946236559136</v>
+        <f>A2*100/$J$2</f>
+        <v>34.408602150537632</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:G4" si="0">B2*100/$I$2</f>
-        <v>37.634408602150536</v>
+        <f t="shared" ref="B4:H4" si="0">B2*100/$J$2</f>
+        <v>36.55913978494624</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>9.67741935483871</v>
+        <v>12.903225806451612</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>3.225806451612903</v>
+        <v>4.301075268817204</v>
       </c>
       <c r="E4" s="1" t="e">
         <f t="shared" si="0"/>
@@ -492,14 +504,18 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>4.301075268817204</v>
-      </c>
-      <c r="G4" s="1">
+        <v>3.225806451612903</v>
+      </c>
+      <c r="G4" s="2" t="e">
         <f t="shared" si="0"/>
-        <v>5.376344086021505</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>8.6021505376344081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -511,7 +527,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>44</v>
       </c>
@@ -519,7 +535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>A9*100/D8</f>
         <v>47.826086956521742</v>
@@ -529,11 +545,11 @@
         <v>52.173913043478258</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Complete federal-state analysis for three recent elections
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A13F4A-DD28-4E2B-BAD8-CACB0DE26469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE59E65-5F4B-4622-B2B3-895E74BD13C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14190" yWindow="12255" windowWidth="28800" windowHeight="15435" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="150" yWindow="4890" windowWidth="27855" windowHeight="15435" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,58 +453,59 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>35</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="B2" s="2">
-        <v>36</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="C2" s="2">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D2" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="E2" s="2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2" s="2">
-        <v>3</v>
+      <c r="F2" s="2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="G2" s="2" t="e">
         <v>#N/A</v>
       </c>
       <c r="H2" s="2">
-        <v>8</v>
+        <f>100-11.9-A2-B2-C2</f>
+        <v>10.399999999999995</v>
       </c>
       <c r="J2">
         <f>SUMIF(A2:H2,"&gt;0")</f>
-        <v>100</v>
+        <v>88.1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$J$2</f>
-        <v>35</v>
+        <v>36.54937570942112</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:H4" si="0">B2*100/$J$2</f>
-        <v>36</v>
+        <v>40.068104426787741</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
+        <v>11.577752553916003</v>
+      </c>
+      <c r="D4" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>#N/A</v>
       </c>
       <c r="E4" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="1" t="e">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>#N/A</v>
       </c>
       <c r="G4" s="2" t="e">
         <f t="shared" si="0"/>
@@ -512,7 +513,7 @@
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11.804767309875137</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix various issues pre/post 2023nsw
-Pollster analysis: adjustment for federal
election being overweighted for state results
-Pollster analysis: fix for elections being
weighter more when distant in time (should of
course be when closer in time.)
-Fix SFF not being recognised in 2019nsw
-Better estimations for live seat preference flows/exhaust rates
-Better nowcast date handling
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE59E65-5F4B-4622-B2B3-895E74BD13C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F16CDA-99D4-4F7C-BD87-BEF4FC27CA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="4890" windowWidth="27855" windowHeight="15435" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="21450" yWindow="5310" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>LNP</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>DEM</t>
+  </si>
+  <si>
+    <t>DLP</t>
   </si>
 </sst>
 </file>
@@ -96,9 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,109 +415,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="9.140625" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="B2" s="2">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D2" s="2" t="e">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E2" s="2" t="e">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2" s="2" t="e">
+      <c r="H2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G2" s="2" t="e">
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(A2:I2,"&gt;0")</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A2*100/$K$2</f>
+        <v>31.578947368421051</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
+        <v>34.736842105263158</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>14.736842105263158</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6.3157894736842106</v>
+      </c>
+      <c r="E4" t="e">
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="H2" s="2">
-        <f>100-11.9-A2-B2-C2</f>
-        <v>10.399999999999995</v>
-      </c>
-      <c r="J2">
-        <f>SUMIF(A2:H2,"&gt;0")</f>
-        <v>88.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>A2*100/$J$2</f>
-        <v>36.54937570942112</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" ref="B4:H4" si="0">B2*100/$J$2</f>
-        <v>40.068104426787741</v>
-      </c>
-      <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>11.577752553916003</v>
-      </c>
-      <c r="D4" s="1" t="e">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2.1052631578947367</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="E4" s="1" t="e">
+      <c r="H4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G4" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="0"/>
-        <v>11.804767309875137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>10.526315789473685</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -525,34 +532,29 @@
       </c>
       <c r="D8">
         <f>SUM(A9:B9)</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B9">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f>A9*100/D8</f>
-        <v>44.943820224719104</v>
-      </c>
-      <c r="B10" s="2">
+        <v>44.210526315789473</v>
+      </c>
+      <c r="B10">
         <f>B9*100/D8</f>
-        <v>55.056179775280896</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
+        <v>55.789473684210527</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix projection detail creation not working properly.
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA623158-2243-4989-9BB2-0C5CBBFBF0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B700ED5D-6668-4595-A1DE-7273F38024DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14610" yWindow="6045" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="12540" yWindow="4665" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,16 +462,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -486,29 +486,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>25.252525252525253</v>
+        <v>32.258064516129032</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>45.454545454545453</v>
+        <v>34.408602150537632</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
+        <v>15.053763440860216</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>3.0303030303030303</v>
+        <v>7.5268817204301079</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -516,7 +516,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2.0202020202020203</v>
+        <v>2.150537634408602</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -528,25 +528,25 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>13.131313131313131</v>
+        <v>8.6021505376344081</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>25.252525252525253</v>
+        <v>32.258064516129032</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>45.454545454545453</v>
+        <v>34.408602150537632</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
+        <v>15.053763440860216</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>3.0303030303030303</v>
+        <v>7.5268817204301079</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -554,7 +554,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.0202020202020203</v>
+        <v>2.150537634408602</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>13.131313131313131</v>
+        <v>8.6021505376344081</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>64.056616161616162</v>
+        <v>55.555591397849462</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -621,17 +621,17 @@
         <v>42</v>
       </c>
       <c r="B10">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>44.210526315789473</v>
+        <v>44.680851063829785</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>55.789473684210527</v>
+        <v>55.319148936170215</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Make trend use pollster analysis marked for it
Also make pollster analysis treat LIB/LNP in the same category.
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AB5E78-A23C-43E9-AB5A-465F85EC5D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E187E1C6-604A-459F-9768-18B8E42643C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27045" yWindow="3900" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="14685" yWindow="8250" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,91 +464,91 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>31</v>
-      </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="C2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H2" t="e">
-        <v>#N/A</v>
+      <c r="F2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>35.789473684210527</v>
+        <v>34.482758620689658</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>32.631578947368418</v>
-      </c>
-      <c r="C4">
+        <v>47.126436781609193</v>
+      </c>
+      <c r="C4" t="e">
         <f t="shared" si="0"/>
-        <v>13.684210526315789</v>
-      </c>
-      <c r="D4">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" t="e">
         <f t="shared" si="0"/>
-        <v>6.3157894736842106</v>
+        <v>#N/A</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="e">
         <f t="shared" si="0"/>
-        <v>2.1052631578947367</v>
-      </c>
-      <c r="G4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" t="e">
+        <v>18.390804597701148</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>9.473684210526315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>35.789473684210527</v>
+        <v>34.482758620689658</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>32.631578947368418</v>
+        <v>47.126436781609193</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>13.684210526315789</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>6.3157894736842106</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -556,11 +556,11 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.1052631578947367</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.390804597701148</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>9.473684210526315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>52.633842105263163</v>
+        <v>47.126436781609193</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix bug causing pollster biases to be ignored.
Bug was introduced in the recent overhaul of the pollster analysis system.
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E187E1C6-604A-459F-9768-18B8E42643C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332D0340-C669-4A0E-B18A-714ECD335A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14685" yWindow="8250" windowWidth="23115" windowHeight="15090" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="2220" yWindow="1845" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>LNP</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>DLP</t>
+  </si>
+  <si>
+    <t>OPV</t>
+  </si>
+  <si>
+    <t>&lt;- pref flow</t>
+  </si>
+  <si>
+    <t>&lt;- survival</t>
   </si>
 </sst>
 </file>
@@ -425,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,91 +473,91 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>35</v>
+      </c>
+      <c r="B2">
         <v>30</v>
       </c>
-      <c r="B2">
-        <v>41</v>
-      </c>
-      <c r="C2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#N/A</v>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2" t="e">
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G2">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>34.482758620689658</v>
+        <v>36.842105263157897</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>47.126436781609193</v>
-      </c>
-      <c r="C4" t="e">
+        <v>31.578947368421051</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" t="e">
+        <v>13.684210526315789</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>7.3684210526315788</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4" t="e">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2.1052631578947367</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="G4">
+      <c r="H4" t="e">
         <f t="shared" si="0"/>
-        <v>18.390804597701148</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.4210526315789469</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>34.482758620689658</v>
+        <v>36.842105263157897</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>47.126436781609193</v>
+        <v>31.578947368421051</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.684210526315789</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.3684210526315788</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -556,11 +565,11 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.1052631578947367</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>18.390804597701148</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
@@ -568,7 +577,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.4210526315789469</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -603,7 +612,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>47.126436781609193</v>
+        <v>51.378052631578953</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -620,25 +629,158 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>48.421052631578945</v>
+        <v>50.526315789473685</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>51.578947368421055</v>
+        <v>49.473684210526315</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>41.6</v>
+      </c>
+      <c r="B24">
+        <v>42.25</v>
+      </c>
+      <c r="C24">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>60</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>70</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>40</v>
+      </c>
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f>SUMPRODUCT(A24:I24,A25:I25,A26:I26)/(SUMPRODUCT(A24:I24,A25:I25))</f>
+        <v>50.922172332691893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can suspend trend model via text file
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77BB4A-28C6-45AF-A680-765217883430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E4D44-7DA4-4707-B776-3E7967A7A27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12690" yWindow="8730" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="18690" yWindow="9495" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,16 +473,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -497,29 +497,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>36.363636363636367</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>30.303030303030305</v>
+        <v>32.291666666666664</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>14.141414141414142</v>
+        <v>11.458333333333334</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>7.0707070707070709</v>
+        <v>9.375</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -527,7 +527,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1.0101010101010102</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -539,25 +539,25 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>36.363636363636367</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>30.303030303030305</v>
+        <v>32.291666666666664</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>14.141414141414142</v>
+        <v>11.458333333333334</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>7.0707070707070709</v>
+        <v>9.375</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>1.0101010101010102</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -577,7 +577,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>51.450202020202028</v>
+        <v>51.017760416666661</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -624,25 +624,25 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>49</v>
+      </c>
+      <c r="B10">
         <v>47</v>
-      </c>
-      <c r="B10">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>49.473684210526315</v>
+        <v>51.041666666666664</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>50.526315789473685</v>
+        <v>48.958333333333336</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix some MRP-related issues
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E4D44-7DA4-4707-B776-3E7967A7A27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF32A9-A02B-4D8A-89AF-ABC47478B3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18690" yWindow="9495" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="19785" yWindow="1725" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,16 +473,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>31</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -501,25 +501,25 @@
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>36.458333333333336</v>
+        <v>34.042553191489361</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>32.291666666666664</v>
+        <v>32.978723404255319</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>11.458333333333334</v>
+        <v>13.829787234042554</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>9.375</v>
+        <v>8.5106382978723403</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -527,7 +527,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1.0416666666666667</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -539,25 +539,25 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>9.375</v>
+        <v>9.5744680851063837</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>36.458333333333336</v>
+        <v>34.042553191489361</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>32.291666666666664</v>
+        <v>32.978723404255319</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>11.458333333333334</v>
+        <v>13.829787234042554</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>9.375</v>
+        <v>8.5106382978723403</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>1.0416666666666667</v>
+        <v>1.0638297872340425</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -577,7 +577,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>9.375</v>
+        <v>9.5744680851063837</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>51.017760416666661</v>
+        <v>53.54803191489362</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -624,25 +624,25 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>51.041666666666664</v>
+        <v>48.936170212765958</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>48.958333333333336</v>
+        <v>51.063829787234042</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix certain candidate types disappearing from simulations
(affected: "significant" candidates belonging to a named party that doesn't have a calculated vote trend)
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF32A9-A02B-4D8A-89AF-ABC47478B3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BD5920-4590-44D3-9DE6-0F419F06A52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19785" yWindow="1725" windowWidth="23115" windowHeight="19335" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="15270" yWindow="2895" windowWidth="20910" windowHeight="17025" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>LNP</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>&lt;- survival</t>
+  </si>
+  <si>
+    <t>qld</t>
   </si>
 </sst>
 </file>
@@ -434,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71DF0CB-5BDB-44EF-865D-4A87CF8BD5AA}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,24 +474,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>32</v>
+        <v>35.89</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>39.57</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>7.12</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2.52</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -497,29 +500,30 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <f>100-35.89-39.57-9.47-7.12-2.52</f>
+        <v>5.4299999999999979</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>34.042553191489361</v>
+        <v>35.89</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>32.978723404255319</v>
+        <v>39.57</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>13.829787234042554</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>8.5106382978723403</v>
+        <v>7.12</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -527,7 +531,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>1.0638297872340425</v>
+        <v>2.52</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -539,25 +543,30 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>9.5744680851063837</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.4299999999999979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>34.042553191489361</v>
+        <v>35.89</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>32.978723404255319</v>
+        <v>39.57</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>13.829787234042554</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>8.5106382978723403</v>
+        <v>7.12</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -565,7 +574,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>1.0638297872340425</v>
+        <v>2.52</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -577,10 +586,10 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>9.5744680851063837</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5.4299999999999979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -588,16 +597,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0.85755000000000003</v>
+        <f>IF($M$5="qld",0.801,0.85755)</f>
+        <v>0.80100000000000005</v>
       </c>
       <c r="D7" s="1">
-        <v>0.35699999999999998</v>
+        <f>IF($M$5="qld",0.338,0.357)</f>
+        <v>0.33800000000000002</v>
       </c>
       <c r="E7" s="1">
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
-        <v>0.38100000000000001</v>
+        <f>IF($M$5="qld",0.474,0.381)</f>
+        <v>0.47399999999999998</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -606,16 +618,17 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <f>IF($M$5="qld",0.45,0.55)</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>53.54803191489362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53.200009999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -624,28 +637,28 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>48.936170212765958</v>
+        <v>48.958333333333336</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>51.063829787234042</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>51.041666666666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
prepare for 2024qld live forecast
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BD5920-4590-44D3-9DE6-0F419F06A52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC99C33-D57C-43B0-84A1-73CF49DC4A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15270" yWindow="2895" windowWidth="20910" windowHeight="17025" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="21180" yWindow="8085" windowWidth="20910" windowHeight="17025" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>&lt;- survival</t>
   </si>
   <si>
-    <t>qld</t>
+    <t>fed</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,22 +476,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>35.89</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>39.57</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>9.4700000000000006</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>7.12</v>
+        <v>7</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
       <c r="F2">
-        <v>2.52</v>
+        <v>2</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -500,30 +500,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <f>100-35.89-39.57-9.47-7.12-2.52</f>
-        <v>5.4299999999999979</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>35.89</v>
+        <v>37.634408602150536</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>39.57</v>
+        <v>30.107526881720432</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>9.4700000000000006</v>
+        <v>12.903225806451612</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>7.12</v>
+        <v>7.5268817204301079</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -531,7 +530,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2.52</v>
+        <v>2.150537634408602</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -543,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>5.4299999999999979</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -554,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>35.89</v>
+        <v>37.634408602150536</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>39.57</v>
+        <v>30.107526881720432</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>9.4700000000000006</v>
+        <v>12.903225806451612</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>7.12</v>
+        <v>7.5268817204301079</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -574,7 +573,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.52</v>
+        <v>2.150537634408602</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -586,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>5.4299999999999979</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -598,18 +597,18 @@
       </c>
       <c r="C7" s="1">
         <f>IF($M$5="qld",0.801,0.85755)</f>
-        <v>0.80100000000000005</v>
+        <v>0.85755000000000003</v>
       </c>
       <c r="D7" s="1">
         <f>IF($M$5="qld",0.338,0.357)</f>
-        <v>0.33800000000000002</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="E7" s="1">
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
         <f>IF($M$5="qld",0.474,0.381)</f>
-        <v>0.47399999999999998</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -619,13 +618,13 @@
       </c>
       <c r="I7" s="1">
         <f>IF($M$5="qld",0.45,0.55)</f>
-        <v>0.45</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>53.200009999999999</v>
+        <v>50.001720430107525</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -637,25 +636,25 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>48.958333333333336</v>
+        <v>51.063829787234042</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>51.041666666666664</v>
+        <v>48.936170212765958</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
first pass at including nats
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC99C33-D57C-43B0-84A1-73CF49DC4A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B1426E-CD80-4627-AD30-9339EB24FAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="8085" windowWidth="20910" windowHeight="17025" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="10935" yWindow="4410" windowWidth="20910" windowHeight="17010" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,19 +479,19 @@
         <v>35</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -500,29 +500,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>37.634408602150536</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>30.107526881720432</v>
+        <v>31.25</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>12.903225806451612</v>
+        <v>13.541666666666666</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>7.5268817204301079</v>
+        <v>6.25</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -530,7 +530,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2.150537634408602</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>9.67741935483871</v>
+        <v>11.458333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -553,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>37.634408602150536</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>30.107526881720432</v>
+        <v>31.25</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>12.903225806451612</v>
+        <v>13.541666666666666</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>7.5268817204301079</v>
+        <v>6.25</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.150537634408602</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>9.67741935483871</v>
+        <v>11.458333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>50.001720430107525</v>
+        <v>51.792864583333341</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -644,17 +644,17 @@
         <v>48</v>
       </c>
       <c r="B10">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>51.063829787234042</v>
+        <v>50.526315789473685</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>48.936170212765958</v>
+        <v>49.473684210526315</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes to successfully rerun 2022fed live simulation.
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B1426E-CD80-4627-AD30-9339EB24FAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DE4B8E-D359-4F72-88A2-5E01E7448AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="4410" windowWidth="20910" windowHeight="17010" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="13995" yWindow="4500" windowWidth="20910" windowHeight="17010" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,10 +482,10 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -500,7 +500,7 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
@@ -518,11 +518,11 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>13.541666666666666</v>
+        <v>12.5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>6.25</v>
+        <v>9.375</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>11.458333333333334</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -561,11 +561,11 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>13.541666666666666</v>
+        <v>12.5</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>9.375</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>11.458333333333334</v>
+        <v>9.375</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>51.792864583333341</v>
+        <v>50.869374999999998</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -636,12 +636,12 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>47</v>
@@ -650,11 +650,11 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>50.526315789473685</v>
+        <v>51.041666666666664</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>49.473684210526315</v>
+        <v>48.958333333333336</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increase fed-state correlation median in line with recent elections
also update user-agent header, add booths for 2026vic fed-state correlations
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB84B1DF-ACFF-4307-8272-07673FCC649E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E153C8-1394-4809-A1CF-82206E1074F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17595" yWindow="4410" windowWidth="20910" windowHeight="17010" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="15435" yWindow="3765" windowWidth="23070" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,22 +476,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F2">
-        <v>2</v>
+      <c r="F2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -500,37 +500,37 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>35.789473684210527</v>
+        <v>32.978723404255319</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>31.578947368421051</v>
+        <v>35.106382978723403</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>12.631578947368421</v>
+        <v>15.957446808510639</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>9.473684210526315</v>
+        <v>10.638297872340425</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="e">
         <f t="shared" si="0"/>
-        <v>2.1052631578947367</v>
+        <v>#N/A</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>8.4210526315789469</v>
+        <v>5.3191489361702127</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -553,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>35.789473684210527</v>
+        <v>32.978723404255319</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>31.578947368421051</v>
+        <v>35.106382978723403</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>12.631578947368421</v>
+        <v>15.957446808510639</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>9.473684210526315</v>
+        <v>10.638297872340425</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>2.1052631578947367</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>8.4210526315789469</v>
+        <v>5.3191489361702127</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -596,19 +596,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <f>IF($M$5="qld",0.801,0.85755)</f>
-        <v>0.85755000000000003</v>
+        <f>IF($M$5="qld",0.801,0.8819)</f>
+        <v>0.88190000000000002</v>
       </c>
       <c r="D7" s="1">
-        <f>IF($M$5="qld",0.338,0.357)</f>
-        <v>0.35699999999999998</v>
+        <f>IF($M$5="qld",0.338,0.255)</f>
+        <v>0.255</v>
       </c>
       <c r="E7" s="1">
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
-        <f>IF($M$5="qld",0.474,0.381)</f>
-        <v>0.38100000000000001</v>
+        <f>IF($M$5="qld",0.474,0.3619)</f>
+        <v>0.3619</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -617,14 +617,14 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f>IF($M$5="qld",0.45,0.55)</f>
-        <v>0.55000000000000004</v>
+        <f>IF($M$5="qld",0.45,0.545)</f>
+        <v>0.54500000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>51.226947368421065</v>
+        <v>54.790957446808505</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix error in live simulations from NAT vote share
Nationals vote share became NaN when no coalition votes recorded.
This fix sets it to a null optional instead, which is handled properly (ignored with baseline NAT share used)
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E153C8-1394-4809-A1CF-82206E1074F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFED2EA-6418-47C7-AC3D-90DB44DD9D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15435" yWindow="3765" windowWidth="23070" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="7605" yWindow="4350" windowWidth="23070" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,16 +476,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
         <v>31</v>
       </c>
-      <c r="B2">
-        <v>33</v>
-      </c>
       <c r="C2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -500,29 +500,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>32.978723404255319</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>35.106382978723403</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>15.957446808510639</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>10.638297872340425</v>
+        <v>13</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>5.3191489361702127</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -553,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>32.978723404255319</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>35.106382978723403</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>15.957446808510639</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>10.638297872340425</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>5.3191489361702127</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>54.790957446808505</v>
+        <v>51.180199999999999</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
various fixes & improvement to live simulations + logging
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFED2EA-6418-47C7-AC3D-90DB44DD9D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A91A8-1DC5-4670-976D-97555B2812AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="4350" windowWidth="23070" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="13755" yWindow="1905" windowWidth="23640" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,13 +476,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>13</v>
@@ -500,29 +500,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>30</v>
+        <v>25.742574257425744</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>31</v>
+        <v>34.653465346534652</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12.871287128712872</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12.871287128712872</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>13.861386138613861</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -553,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>30</v>
+        <v>25.742574257425744</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>31</v>
+        <v>34.653465346534652</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>12.871287128712872</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12.871287128712872</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>13.861386138613861</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>51.180199999999999</v>
+        <v>56.841287128712871</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -636,25 +636,25 @@
       </c>
       <c r="D9">
         <f>SUM(A10:B10)</f>
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10*100/D9</f>
-        <v>49.473684210526315</v>
+        <v>47.872340425531917</v>
       </c>
       <c r="B11">
         <f>B10*100/D9</f>
-        <v>50.526315789473685</v>
+        <v>52.127659574468083</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -698,16 +698,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>37.92</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>46.92</v>
+        <v>34</v>
       </c>
       <c r="C24">
-        <v>7.99</v>
+        <v>11</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -722,8 +722,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f>1.89+0.6+4.68</f>
-        <v>7.17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -734,10 +733,10 @@
         <v>100</v>
       </c>
       <c r="C25">
-        <v>51</v>
+        <v>66.8</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -752,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J25" t="s">
         <v>12</v>
@@ -766,10 +765,10 @@
         <v>100</v>
       </c>
       <c r="C26">
-        <v>60.8</v>
+        <v>89.1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -784,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>44.62</v>
+        <v>52.8</v>
       </c>
       <c r="J26" t="s">
         <v>11</v>
@@ -793,7 +792,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I28">
         <f>SUMPRODUCT(A24:I24,A25:I25,A26:I26)/(SUMPRODUCT(A24:I24,A25:I25))</f>
-        <v>55.123989150020094</v>
+        <v>58.909354578354034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update NSW federal-state transposed vote
+fixes to booth/vote type bias calcuations
+update other data
</commit_message>
<xml_diff>
--- a/Poll normaliser.xlsx
+++ b/Poll normaliser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djhir\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A91A8-1DC5-4670-976D-97555B2812AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DCD380-6DCB-4789-A946-C7489F8C2A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13755" yWindow="1905" windowWidth="23640" windowHeight="17940" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
+    <workbookView xWindow="16200" yWindow="5565" windowWidth="24345" windowHeight="17730" xr2:uid="{6D0FA6D2-DD42-4A2B-A7FB-8B25D0B69908}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,16 +476,16 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>35</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" t="e">
         <v>#N/A</v>
@@ -500,29 +500,29 @@
         <v>#N/A</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <f>SUMIF(A2:I2,"&gt;0")</f>
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A2*100/$K$2</f>
-        <v>25.742574257425744</v>
+        <v>24.242424242424242</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:I4" si="0">B2*100/$K$2</f>
-        <v>34.653465346534652</v>
+        <v>35.353535353535356</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>12.871287128712872</v>
+        <v>6.0606060606060606</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>12.871287128712872</v>
+        <v>16.161616161616163</v>
       </c>
       <c r="E4" t="e">
         <f t="shared" si="0"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>13.861386138613861</v>
+        <v>18.181818181818183</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -553,19 +553,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>_xlfn.IFNA(A4,0)</f>
-        <v>25.742574257425744</v>
+        <v>24.242424242424242</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:I6" si="1">_xlfn.IFNA(B4,0)</f>
-        <v>34.653465346534652</v>
+        <v>35.353535353535356</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>12.871287128712872</v>
+        <v>6.0606060606060606</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>12.871287128712872</v>
+        <v>16.161616161616163</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -585,7 +585,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>13.861386138613861</v>
+        <v>18.181818181818183</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K8">
         <f>SUMPRODUCT(A6:I6,A7:I7)</f>
-        <v>56.841287128712871</v>
+        <v>54.728686868686879</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>